<commit_message>
notes L1 bio Dimitry et Matthieu : OK
</commit_message>
<xml_diff>
--- a/1.05A.xlsx
+++ b/1.05A.xlsx
@@ -2390,17 +2390,17 @@
   </sheetPr>
   <dimension ref="A1:E475"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D124" activeCellId="0" sqref="D124"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D265" activeCellId="0" sqref="D265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="250" min="4" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="251" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="250" min="4" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="251" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2678,7 +2678,9 @@
       <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="n">
+        <v>1.5</v>
+      </c>
       <c r="E20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2704,7 +2706,9 @@
       <c r="C22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="n">
+        <v>10.25</v>
+      </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2853,7 +2857,9 @@
       <c r="C33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="n">
+        <v>2</v>
+      </c>
       <c r="E33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2894,7 +2900,9 @@
       <c r="C36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="n">
+        <v>9</v>
+      </c>
       <c r="E36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3187,7 +3195,9 @@
       <c r="C57" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="3" t="n">
+        <v>4.25</v>
+      </c>
       <c r="E57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3299,7 +3309,9 @@
       <c r="C65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D65" s="3"/>
+      <c r="D65" s="3" t="n">
+        <v>9.5</v>
+      </c>
       <c r="E65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3413,7 +3425,9 @@
       <c r="C73" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D73" s="3"/>
+      <c r="D73" s="3" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3484,7 +3498,9 @@
       <c r="C78" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D78" s="3"/>
+      <c r="D78" s="3" t="n">
+        <v>7.75</v>
+      </c>
       <c r="E78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3523,7 +3539,9 @@
       <c r="C81" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D81" s="3"/>
+      <c r="D81" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="E81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3592,7 +3610,9 @@
       <c r="C86" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D86" s="3"/>
+      <c r="D86" s="3" t="n">
+        <v>6.5</v>
+      </c>
       <c r="E86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3650,7 +3670,9 @@
       <c r="C90" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D90" s="3"/>
+      <c r="D90" s="3" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3745,7 +3767,9 @@
       <c r="C97" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D97" s="3"/>
+      <c r="D97" s="3" t="n">
+        <v>7.75</v>
+      </c>
       <c r="E97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3887,7 +3911,9 @@
       <c r="C107" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D107" s="3"/>
+      <c r="D107" s="3" t="n">
+        <v>1.25</v>
+      </c>
       <c r="E107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4051,7 +4077,9 @@
       <c r="C119" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D119" s="3"/>
+      <c r="D119" s="3" t="n">
+        <v>0.5</v>
+      </c>
       <c r="E119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4150,7 +4178,9 @@
       <c r="C126" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D126" s="3"/>
+      <c r="D126" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="E126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4236,7 +4266,9 @@
       <c r="C132" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D132" s="3"/>
+      <c r="D132" s="3" t="n">
+        <v>6.25</v>
+      </c>
       <c r="E132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4357,7 +4389,9 @@
       <c r="C141" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D141" s="3"/>
+      <c r="D141" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="E141" s="3"/>
     </row>
     <row r="142" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4439,7 +4473,9 @@
       <c r="C147" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D147" s="3"/>
+      <c r="D147" s="3" t="n">
+        <v>7.5</v>
+      </c>
       <c r="E147" s="3"/>
     </row>
     <row r="148" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4480,7 +4516,9 @@
       <c r="C150" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D150" s="3"/>
+      <c r="D150" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="E150" s="3"/>
     </row>
     <row r="151" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4605,7 +4643,9 @@
       <c r="C159" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="D159" s="3"/>
+      <c r="D159" s="3" t="n">
+        <v>10.5</v>
+      </c>
       <c r="E159" s="3"/>
     </row>
     <row r="160" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4700,7 +4740,9 @@
       <c r="C166" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D166" s="3"/>
+      <c r="D166" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="E166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4782,7 +4824,9 @@
       <c r="C172" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D172" s="3"/>
+      <c r="D172" s="3" t="n">
+        <v>10.5</v>
+      </c>
       <c r="E172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4808,7 +4852,9 @@
       <c r="C174" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D174" s="3"/>
+      <c r="D174" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="E174" s="3"/>
     </row>
     <row r="175" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4959,7 +5005,9 @@
       <c r="C185" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D185" s="3"/>
+      <c r="D185" s="3" t="n">
+        <v>4.25</v>
+      </c>
       <c r="E185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5080,7 +5128,9 @@
       <c r="C194" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D194" s="3"/>
+      <c r="D194" s="3" t="n">
+        <v>9</v>
+      </c>
       <c r="E194" s="3"/>
     </row>
     <row r="195" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5121,7 +5171,9 @@
       <c r="C197" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D197" s="3"/>
+      <c r="D197" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="E197" s="3"/>
     </row>
     <row r="198" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5175,7 +5227,9 @@
       <c r="C201" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="D201" s="3"/>
+      <c r="D201" s="3" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E201" s="3"/>
     </row>
     <row r="202" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5339,7 +5393,9 @@
       <c r="C213" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="D213" s="3"/>
+      <c r="D213" s="3" t="n">
+        <v>6.5</v>
+      </c>
       <c r="E213" s="3"/>
     </row>
     <row r="214" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5408,7 +5464,9 @@
       <c r="C218" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="D218" s="3"/>
+      <c r="D218" s="3" t="n">
+        <v>4</v>
+      </c>
       <c r="E218" s="3"/>
     </row>
     <row r="219" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5421,7 +5479,9 @@
       <c r="C219" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D219" s="3"/>
+      <c r="D219" s="3" t="n">
+        <v>5.5</v>
+      </c>
       <c r="E219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5494,7 +5554,9 @@
       <c r="C224" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="D224" s="3"/>
+      <c r="D224" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="E224" s="3"/>
     </row>
     <row r="225" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5770,7 +5832,9 @@
       <c r="C244" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D244" s="3"/>
+      <c r="D244" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="E244" s="3"/>
     </row>
     <row r="245" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5964,7 +6028,9 @@
       <c r="C258" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="D258" s="3"/>
+      <c r="D258" s="3" t="n">
+        <v>4.75</v>
+      </c>
       <c r="E258" s="3"/>
     </row>
     <row r="259" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6046,7 +6112,9 @@
       <c r="C264" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D264" s="3"/>
+      <c r="D264" s="3" t="n">
+        <v>7.25</v>
+      </c>
       <c r="E264" s="3"/>
     </row>
     <row r="265" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6059,7 +6127,9 @@
       <c r="C265" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="D265" s="3"/>
+      <c r="D265" s="3" t="n">
+        <v>3.5</v>
+      </c>
       <c r="E265" s="3"/>
     </row>
     <row r="266" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6072,7 +6142,9 @@
       <c r="C266" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D266" s="3"/>
+      <c r="D266" s="3" t="n">
+        <v>3.75</v>
+      </c>
       <c r="E266" s="3"/>
     </row>
     <row r="267" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6184,7 +6256,9 @@
       <c r="C274" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D274" s="3"/>
+      <c r="D274" s="3" t="n">
+        <v>8.75</v>
+      </c>
       <c r="E274" s="3"/>
     </row>
     <row r="275" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6322,7 +6396,9 @@
       <c r="C284" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D284" s="3"/>
+      <c r="D284" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="E284" s="3"/>
     </row>
     <row r="285" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6348,7 +6424,9 @@
       <c r="C286" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="D286" s="3"/>
+      <c r="D286" s="3" t="n">
+        <v>2.5</v>
+      </c>
       <c r="E286" s="3"/>
     </row>
     <row r="287" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6445,7 +6523,9 @@
       <c r="C293" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="D293" s="3"/>
+      <c r="D293" s="3" t="n">
+        <v>5.75</v>
+      </c>
       <c r="E293" s="3"/>
     </row>
     <row r="294" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6458,7 +6538,9 @@
       <c r="C294" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="D294" s="3"/>
+      <c r="D294" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="E294" s="3"/>
     </row>
     <row r="295" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6497,7 +6579,9 @@
       <c r="C297" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D297" s="3"/>
+      <c r="D297" s="3" t="n">
+        <v>15</v>
+      </c>
       <c r="E297" s="3"/>
     </row>
     <row r="298" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6538,7 +6622,9 @@
       <c r="C300" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="D300" s="3"/>
+      <c r="D300" s="3" t="n">
+        <v>12.25</v>
+      </c>
       <c r="E300" s="3"/>
     </row>
     <row r="301" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6551,7 +6637,9 @@
       <c r="C301" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="D301" s="3"/>
+      <c r="D301" s="3" t="n">
+        <v>6</v>
+      </c>
       <c r="E301" s="3"/>
     </row>
     <row r="302" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6762,7 +6850,9 @@
       <c r="C316" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="D316" s="3"/>
+      <c r="D316" s="3" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E316" s="3"/>
     </row>
     <row r="317" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6788,7 +6878,9 @@
       <c r="C318" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="D318" s="3"/>
+      <c r="D318" s="3" t="n">
+        <v>1.5</v>
+      </c>
       <c r="E318" s="3"/>
     </row>
     <row r="319" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6883,7 +6975,9 @@
       <c r="C325" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="D325" s="3"/>
+      <c r="D325" s="3" t="n">
+        <v>2.5</v>
+      </c>
       <c r="E325" s="3"/>
     </row>
     <row r="326" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6909,7 +7003,9 @@
       <c r="C327" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="D327" s="3"/>
+      <c r="D327" s="3" t="n">
+        <v>3.5</v>
+      </c>
       <c r="E327" s="3"/>
     </row>
     <row r="328" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7146,7 +7242,9 @@
       <c r="C344" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="D344" s="3"/>
+      <c r="D344" s="3" t="n">
+        <v>1.75</v>
+      </c>
       <c r="E344" s="3"/>
     </row>
     <row r="345" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7185,7 +7283,9 @@
       <c r="C347" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="D347" s="3"/>
+      <c r="D347" s="3" t="n">
+        <v>3.25</v>
+      </c>
       <c r="E347" s="3"/>
     </row>
     <row r="348" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7198,7 +7298,9 @@
       <c r="C348" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D348" s="3"/>
+      <c r="D348" s="3" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E348" s="3"/>
     </row>
     <row r="349" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7280,7 +7382,9 @@
       <c r="C354" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D354" s="3"/>
+      <c r="D354" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="E354" s="3"/>
     </row>
     <row r="355" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7319,7 +7423,9 @@
       <c r="C357" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D357" s="3"/>
+      <c r="D357" s="3" t="n">
+        <v>8</v>
+      </c>
       <c r="E357" s="3"/>
     </row>
     <row r="358" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7345,7 +7451,9 @@
       <c r="C359" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D359" s="3"/>
+      <c r="D359" s="3" t="n">
+        <v>3.5</v>
+      </c>
       <c r="E359" s="3"/>
     </row>
     <row r="360" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7401,7 +7509,9 @@
       <c r="C363" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="D363" s="3"/>
+      <c r="D363" s="3" t="n">
+        <v>1.5</v>
+      </c>
       <c r="E363" s="3"/>
     </row>
     <row r="364" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7427,7 +7537,9 @@
       <c r="C365" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="D365" s="3"/>
+      <c r="D365" s="3" t="n">
+        <v>5.25</v>
+      </c>
       <c r="E365" s="3"/>
     </row>
     <row r="366" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7526,7 +7638,9 @@
       <c r="C372" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D372" s="3"/>
+      <c r="D372" s="3" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E372" s="3"/>
     </row>
     <row r="373" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7554,7 +7668,9 @@
       <c r="C374" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D374" s="3"/>
+      <c r="D374" s="3" t="n">
+        <v>2.5</v>
+      </c>
       <c r="E374" s="3"/>
     </row>
     <row r="375" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7582,7 +7698,9 @@
       <c r="C376" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="D376" s="3"/>
+      <c r="D376" s="3" t="n">
+        <v>9</v>
+      </c>
       <c r="E376" s="3"/>
     </row>
     <row r="377" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7690,7 +7808,9 @@
       <c r="C384" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="D384" s="3"/>
+      <c r="D384" s="3" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E384" s="3"/>
     </row>
     <row r="385" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7770,7 +7890,9 @@
       <c r="C390" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D390" s="3"/>
+      <c r="D390" s="3" t="n">
+        <v>10</v>
+      </c>
       <c r="E390" s="3"/>
     </row>
     <row r="391" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7828,7 +7950,9 @@
       <c r="C394" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D394" s="3"/>
+      <c r="D394" s="3" t="n">
+        <v>3.5</v>
+      </c>
       <c r="E394" s="3"/>
     </row>
     <row r="395" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7856,7 +7980,9 @@
       <c r="C396" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="D396" s="3"/>
+      <c r="D396" s="3" t="n">
+        <v>9.75</v>
+      </c>
       <c r="E396" s="3"/>
     </row>
     <row r="397" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8037,7 +8163,9 @@
       <c r="C409" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="D409" s="3"/>
+      <c r="D409" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="E409" s="3"/>
     </row>
     <row r="410" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8190,7 +8318,9 @@
       <c r="C420" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D420" s="3"/>
+      <c r="D420" s="3" t="n">
+        <v>2.5</v>
+      </c>
       <c r="E420" s="3"/>
     </row>
     <row r="421" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8304,7 +8434,9 @@
       <c r="C428" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="D428" s="3"/>
+      <c r="D428" s="3" t="n">
+        <v>12</v>
+      </c>
       <c r="E428" s="3"/>
     </row>
     <row r="429" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8631,7 +8763,9 @@
       <c r="C451" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="D451" s="3"/>
+      <c r="D451" s="3" t="n">
+        <v>7</v>
+      </c>
       <c r="E451" s="3"/>
     </row>
     <row r="452" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8659,7 +8793,9 @@
       <c r="C453" s="2" t="s">
         <v>716</v>
       </c>
-      <c r="D453" s="3"/>
+      <c r="D453" s="3" t="n">
+        <v>13.5</v>
+      </c>
       <c r="E453" s="3"/>
     </row>
     <row r="454" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8741,7 +8877,9 @@
       <c r="C459" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D459" s="3"/>
+      <c r="D459" s="3" t="n">
+        <v>4.25</v>
+      </c>
       <c r="E459" s="3"/>
     </row>
     <row r="460" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8894,7 +9032,9 @@
       <c r="C470" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D470" s="3"/>
+      <c r="D470" s="3" t="n">
+        <v>12</v>
+      </c>
       <c r="E470" s="3"/>
     </row>
     <row r="471" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>